<commit_message>
Reporte plano de actividades por dependencia del organigrama terminado
</commit_message>
<xml_diff>
--- a/src/main/resources/reports/structures/PlainedStructures.xlsx
+++ b/src/main/resources/reports/structures/PlainedStructures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROYECTOS\FORTELECIMEITO Y MODERNIZACION INSTITUCIONAL\APP\Carga-Trabajo-Services\src\main\resources\reports\structures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00FA472-CB62-436E-9562-891D4B616A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEFED0B5-B62E-4D37-88A5-9F31260895FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FC55D6EF-68F2-426F-9839-57243A004983}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{FC55D6EF-68F2-426F-9839-57243A004983}"/>
   </bookViews>
   <sheets>
     <sheet name="Detalle por dependencia" sheetId="2" r:id="rId1"/>
@@ -997,44 +997,44 @@
     <xf numFmtId="2" fontId="18" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1382,7 +1382,7 @@
   <dimension ref="B1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.375" defaultRowHeight="15.75"/>
@@ -1437,19 +1437,19 @@
       <c r="G7" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="26" t="s">
+      <c r="H7" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="I7" s="26" t="s">
+      <c r="I7" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="J7" s="26" t="s">
+      <c r="J7" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="26" t="s">
+      <c r="K7" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="L7" s="26" t="s">
+      <c r="L7" s="38" t="s">
         <v>8</v>
       </c>
       <c r="M7" s="8" t="s">
@@ -1463,26 +1463,26 @@
       <c r="E8" s="35"/>
       <c r="F8" s="35"/>
       <c r="G8" s="33"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="26"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="38"/>
       <c r="M8" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="2:21" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="38" t="s">
+      <c r="D9" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="38" t="s">
+      <c r="E9" s="26" t="s">
         <v>26</v>
       </c>
       <c r="F9" s="1" t="s">
@@ -1568,6 +1568,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="H7:H8"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="G7:G8"/>
@@ -1577,11 +1582,6 @@
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="D7:D8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="H7:H8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1633,7 +1633,7 @@
       <c r="C7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="26" t="s">
+      <c r="D7" s="38" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1642,7 +1642,7 @@
       <c r="C8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="26"/>
+      <c r="D8" s="38"/>
     </row>
     <row r="9" spans="2:4" s="5" customFormat="1" ht="15" customHeight="1">
       <c r="B9" s="13" t="s">

</xml_diff>